<commit_message>
Removal of Data Files
Don't expect raw results to change, and will take up unnecessary space.
</commit_message>
<xml_diff>
--- a/Data/Cr-Hematite_C-Ferrocyanide Redoxotron Results.xlsx
+++ b/Data/Cr-Hematite_C-Ferrocyanide Redoxotron Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\Redoxotron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\ResearchCode\Redoxotron\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -126,10 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1421,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364F44D8-A067-44C1-BC9E-DD5B816A0961}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C25:C26"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,6 +1671,39 @@
         <v>3.3330000000000002</v>
       </c>
       <c r="C21">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>42998.429166666669</v>
+      </c>
+      <c r="B22">
+        <v>1.63</v>
+      </c>
+      <c r="C22">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>43000.432523148149</v>
+      </c>
+      <c r="B23">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="C23">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>43000.68472222222</v>
+      </c>
+      <c r="B24">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="C24">
         <v>2E-3</v>
       </c>
     </row>

</xml_diff>